<commit_message>
representacion en el excel
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49729AB1-6F1E-42AD-B807-28FBF34DE224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -52,9 +53,6 @@
     <t>//valores</t>
   </si>
   <si>
-    <t>**** COMPLETAR ****</t>
-  </si>
-  <si>
     <t>Ejemplo de cómo representar las estructuras de datos según lo visto en teoría:</t>
   </si>
   <si>
@@ -62,13 +60,145 @@
   </si>
   <si>
     <t>¿Para qué se utiliza?: guarda las palabras que se pueden elegidas para jugar wordix</t>
+  </si>
+  <si>
+    <t>"palabraWordix"</t>
+  </si>
+  <si>
+    <t>"jugador"</t>
+  </si>
+  <si>
+    <t>"intentos"</t>
+  </si>
+  <si>
+    <t>"puntaje"</t>
+  </si>
+  <si>
+    <t>"QUESO"</t>
+  </si>
+  <si>
+    <t>"majo"</t>
+  </si>
+  <si>
+    <t>"CINCO"</t>
+  </si>
+  <si>
+    <t>"pepe"</t>
+  </si>
+  <si>
+    <t>"CAJON"</t>
+  </si>
+  <si>
+    <t>"santi"</t>
+  </si>
+  <si>
+    <t>"SILLA"</t>
+  </si>
+  <si>
+    <t>"gaston"</t>
+  </si>
+  <si>
+    <t>"FUEGO"</t>
+  </si>
+  <si>
+    <t>"ely"</t>
+  </si>
+  <si>
+    <t>"HUEVO"</t>
+  </si>
+  <si>
+    <t>"lucas"</t>
+  </si>
+  <si>
+    <t>//claves</t>
+  </si>
+  <si>
+    <t>informacion de la estructura</t>
+  </si>
+  <si>
+    <t>Tipo: multidimensional (arreglo indexado de arreglos asociativos)</t>
+  </si>
+  <si>
+    <t>¿para que se utiliza?: se ultiliza para guardar las partidas de Wordix jugadas por los distintos jugadores</t>
+  </si>
+  <si>
+    <t>"partidas"</t>
+  </si>
+  <si>
+    <t>"puntajeTotal"</t>
+  </si>
+  <si>
+    <t>"victorias"</t>
+  </si>
+  <si>
+    <t>"porcentajeVictorias"</t>
+  </si>
+  <si>
+    <t>"intento1"</t>
+  </si>
+  <si>
+    <t>"intento2"</t>
+  </si>
+  <si>
+    <t>"intento3"</t>
+  </si>
+  <si>
+    <t>"intento4"</t>
+  </si>
+  <si>
+    <t>"intento5"</t>
+  </si>
+  <si>
+    <t>"intento6"</t>
+  </si>
+  <si>
+    <t>$coleccionPartidas=</t>
+  </si>
+  <si>
+    <t>$stats=</t>
+  </si>
+  <si>
+    <t>Tipo: asociativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿para que se utiliza?: se utiliza para almacenar las estadisticas de todas las partidas de un jugador </t>
+  </si>
+  <si>
+    <t>Tipo de datos: el arreglo indexado almacena arreglos asociativos, y estos almacenan datos de tipo string y valores enteros</t>
+  </si>
+  <si>
+    <t>estructura del archivo wordix.php</t>
+  </si>
+  <si>
+    <t>$partida=</t>
+  </si>
+  <si>
+    <t>$palabraWordix</t>
+  </si>
+  <si>
+    <t>$nombreUsuario</t>
+  </si>
+  <si>
+    <t>$nroIntento</t>
+  </si>
+  <si>
+    <t>$puntaje</t>
+  </si>
+  <si>
+    <t>Tipo de datos: almacena datos de tipo string y valores enteros, los cuales son recibidos a travez de variables incluidas en la funcion "jugarWordix"</t>
+  </si>
+  <si>
+    <t>¿para que se utiliza?: se utiliza para guardar los datos de una partida ni bien esta misma finaliza</t>
+  </si>
+  <si>
+    <t>Tipo de datos: almacena datos de tipo string y valores enteros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +233,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,35 +306,488 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F9E2E7-D132-E039-D028-31E062699BFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5819775" y="1757362"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Flecha: hacia abajo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBCF3FB9-D5EC-DECD-B132-551927D4ECBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1685925" y="2867025"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Flecha: hacia abajo 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5333D4FC-3A03-4452-8CB2-CC8E18A7AAF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2600325" y="2886075"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Flecha: hacia abajo 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536C460C-4D84-47B2-975A-4A3685C86302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3505200" y="2886075"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Flecha: hacia abajo 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0406E2AB-A16D-45C2-85DF-89A2EE8E6686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4400550" y="2886075"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Flecha: hacia abajo 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBAAA18A-D753-4123-A2B0-E4EE1CE40C60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5229225" y="2895600"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Flecha: hacia abajo 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D555F9-0187-4166-89AE-B207E0BB29B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6038850" y="2876550"/>
+          <a:ext cx="104775" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -220,7 +825,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -254,6 +859,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -288,9 +894,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,14 +1070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -481,12 +1088,12 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +1119,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,38 +1142,347 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8">
+        <v>5</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>3</v>
+      </c>
+      <c r="E20" s="7">
+        <v>4</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7">
+        <v>0</v>
+      </c>
+      <c r="C21" s="7">
+        <v>15</v>
+      </c>
+      <c r="D21" s="7">
+        <v>13</v>
+      </c>
+      <c r="E21" s="7">
         <v>12</v>
+      </c>
+      <c r="F21" s="7">
+        <v>12</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="N28" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>22</v>
+      </c>
+      <c r="E29" s="7">
+        <v>2</v>
+      </c>
+      <c r="F29" s="10">
+        <v>100</v>
+      </c>
+      <c r="H29" s="7">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7">
+        <v>0</v>
+      </c>
+      <c r="M29" s="7">
+        <v>1</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>